<commit_message>
trying to publish tsv file for survey data
</commit_message>
<xml_diff>
--- a/excel_files/Survey Data.xlsx
+++ b/excel_files/Survey Data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trvrb/Documents/src/tfcb_2019/homeworks/homework01/messy-project-files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/coohleencoombes/Desktop/Git/tfcb-homework01/messy-project-directory/excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A2EF31-99BB-1147-875E-0BF67F65B824}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BECA2E2-2DAB-234D-B1F1-80D140C1FA10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="1400" windowWidth="25120" windowHeight="15580" tabRatio="481" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1960" yWindow="1380" windowWidth="25120" windowHeight="15580" tabRatio="481" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2013" sheetId="1" r:id="rId1"/>
-    <sheet name="2014" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="2014" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="47">
   <si>
     <t>NA</t>
   </si>
@@ -141,15 +142,46 @@
   <si>
     <t>gray cell means my measurement device wasn't calibrated correctly</t>
   </si>
+  <si>
+    <t>plot</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>field season</t>
+  </si>
+  <si>
+    <t>scale calibration</t>
+  </si>
+  <si>
+    <t>Null</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>unit of measure</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>DO</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -162,11 +194,13 @@
     <font>
       <sz val="18"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="28"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="24"/>
@@ -177,16 +211,28 @@
       <b/>
       <sz val="24"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="24"/>
       <color rgb="FF808080"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="24"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -317,7 +363,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -340,6 +386,11 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -797,10 +848,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:AB28"/>
+  <dimension ref="C3:AB176"/>
   <sheetViews>
-    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView topLeftCell="A3" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19:J129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="25" x14ac:dyDescent="0.25"/>
@@ -808,10 +859,12 @@
     <col min="1" max="1" width="18.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="1"/>
     <col min="3" max="3" width="26.1640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.5" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="29.1640625" customWidth="1"/>
+    <col min="5" max="5" width="50.5" customWidth="1"/>
     <col min="6" max="6" width="14.83203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="25.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.5" style="1" customWidth="1"/>
     <col min="12" max="12" width="14.33203125" customWidth="1"/>
     <col min="13" max="13" width="24.83203125" customWidth="1"/>
@@ -966,7 +1019,7 @@
       </c>
       <c r="L8" s="5"/>
       <c r="M8" s="18">
-        <v>41590</v>
+        <v>41505</v>
       </c>
       <c r="N8" s="16">
         <v>9</v>
@@ -1007,7 +1060,7 @@
       </c>
       <c r="L9" s="5"/>
       <c r="M9" s="18">
-        <v>41591</v>
+        <v>41564</v>
       </c>
       <c r="N9" s="16">
         <v>11</v>
@@ -1046,7 +1099,7 @@
       </c>
       <c r="L10" s="5"/>
       <c r="M10" s="18">
-        <v>41591</v>
+        <v>41564</v>
       </c>
       <c r="N10" s="16">
         <v>17</v>
@@ -1085,7 +1138,7 @@
       </c>
       <c r="L11" s="5"/>
       <c r="M11" s="18">
-        <v>41591</v>
+        <v>41618</v>
       </c>
       <c r="N11" s="16">
         <v>14</v>
@@ -1126,7 +1179,7 @@
       </c>
       <c r="L12" s="5"/>
       <c r="M12" s="18">
-        <v>41591</v>
+        <v>41618</v>
       </c>
       <c r="N12" s="16">
         <v>11</v>
@@ -1166,8 +1219,8 @@
         <v>41</v>
       </c>
       <c r="L13" s="5"/>
-      <c r="M13" s="18">
-        <v>41591</v>
+      <c r="M13" s="19">
+        <v>41619</v>
       </c>
       <c r="N13" s="16">
         <v>4</v>
@@ -1290,6 +1343,3387 @@
       <c r="Q18" s="5"/>
     </row>
     <row r="19" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+      <c r="C19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+    </row>
+    <row r="20" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+      <c r="C20" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="18">
+        <v>41471</v>
+      </c>
+      <c r="E20" s="16">
+        <v>2</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J20" s="4">
+        <v>2013</v>
+      </c>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+    </row>
+    <row r="21" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+      <c r="C21" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="18">
+        <v>41471</v>
+      </c>
+      <c r="E21" s="16">
+        <v>7</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21" s="17">
+        <v>33</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J21" s="4">
+        <v>2013</v>
+      </c>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+    </row>
+    <row r="22" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+      <c r="C22" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="18">
+        <v>41471</v>
+      </c>
+      <c r="E22" s="16">
+        <v>3</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J22" s="4">
+        <v>2013</v>
+      </c>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+    </row>
+    <row r="23" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+      <c r="C23" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="18">
+        <v>41471</v>
+      </c>
+      <c r="E23" s="16">
+        <v>1</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J23" s="4">
+        <v>2013</v>
+      </c>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+    </row>
+    <row r="24" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+      <c r="C24" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="18">
+        <v>41473</v>
+      </c>
+      <c r="E24" s="16">
+        <v>3</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="G24" s="17">
+        <v>40</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J24" s="4">
+        <v>2013</v>
+      </c>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
+    </row>
+    <row r="25" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+      <c r="C25" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="18">
+        <v>41473</v>
+      </c>
+      <c r="E25" s="16">
+        <v>7</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="G25" s="17">
+        <v>48</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J25" s="4">
+        <v>2013</v>
+      </c>
+      <c r="L25" s="5"/>
+      <c r="Q25" s="5"/>
+    </row>
+    <row r="26" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+      <c r="C26" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="18">
+        <v>41473</v>
+      </c>
+      <c r="E26" s="16">
+        <v>4</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26" s="17">
+        <v>29</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J26" s="4">
+        <v>2013</v>
+      </c>
+      <c r="L26" s="5"/>
+      <c r="Q26" s="5"/>
+    </row>
+    <row r="27" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+      <c r="C27" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="19">
+        <v>41473</v>
+      </c>
+      <c r="E27" s="20">
+        <v>6</v>
+      </c>
+      <c r="F27" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" s="21">
+        <v>37</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J27" s="4">
+        <v>2013</v>
+      </c>
+      <c r="L27" s="5"/>
+      <c r="Q27" s="5"/>
+    </row>
+    <row r="28" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+      <c r="C28" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="18">
+        <v>41505</v>
+      </c>
+      <c r="E28" s="16">
+        <v>8</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" s="17">
+        <v>52</v>
+      </c>
+      <c r="H28" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="I28" s="24"/>
+      <c r="L28" s="5"/>
+      <c r="Q28" s="5"/>
+    </row>
+    <row r="29" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+      <c r="C29" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="18">
+        <v>41564</v>
+      </c>
+      <c r="E29" s="16">
+        <v>3</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G29" s="17">
+        <v>33</v>
+      </c>
+      <c r="H29" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="I29" s="24"/>
+    </row>
+    <row r="30" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+      <c r="C30" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" s="18">
+        <v>41564</v>
+      </c>
+      <c r="E30" s="16">
+        <v>3</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" s="17">
+        <v>50</v>
+      </c>
+      <c r="H30" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="I30" s="24"/>
+    </row>
+    <row r="31" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+      <c r="C31" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="18">
+        <v>41618</v>
+      </c>
+      <c r="E31" s="16">
+        <v>9</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31" s="17">
+        <v>40</v>
+      </c>
+      <c r="H31" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="I31" s="24"/>
+    </row>
+    <row r="32" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+      <c r="C32" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" s="18">
+        <v>41618</v>
+      </c>
+      <c r="E32" s="16">
+        <v>1</v>
+      </c>
+      <c r="F32" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="G32" s="17">
+        <v>45</v>
+      </c>
+      <c r="H32" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="I32" s="24"/>
+    </row>
+    <row r="33" spans="3:9" ht="30" x14ac:dyDescent="0.3">
+      <c r="C33" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" s="19">
+        <v>41619</v>
+      </c>
+      <c r="E33" s="20">
+        <v>8</v>
+      </c>
+      <c r="F33" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G33" s="21">
+        <v>41</v>
+      </c>
+      <c r="H33" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="I33" s="24"/>
+    </row>
+    <row r="34" spans="3:9" ht="30" x14ac:dyDescent="0.3">
+      <c r="C34" s="23"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
+    </row>
+    <row r="35" spans="3:9" ht="30" x14ac:dyDescent="0.3">
+      <c r="C35" s="23"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
+    </row>
+    <row r="36" spans="3:9" ht="30" x14ac:dyDescent="0.3">
+      <c r="C36" s="23"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="24"/>
+    </row>
+    <row r="37" spans="3:9" ht="30" x14ac:dyDescent="0.3">
+      <c r="C37" s="23"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="24"/>
+      <c r="H37" s="24"/>
+      <c r="I37" s="24"/>
+    </row>
+    <row r="38" spans="3:9" ht="30" x14ac:dyDescent="0.3">
+      <c r="C38" s="23"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="24"/>
+    </row>
+    <row r="39" spans="3:9" ht="30" x14ac:dyDescent="0.3">
+      <c r="C39" s="23"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="24"/>
+      <c r="H39" s="24"/>
+      <c r="I39" s="24"/>
+    </row>
+    <row r="40" spans="3:9" ht="30" x14ac:dyDescent="0.3">
+      <c r="C40" s="23"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="24"/>
+      <c r="H40" s="24"/>
+      <c r="I40" s="24"/>
+    </row>
+    <row r="41" spans="3:9" ht="30" x14ac:dyDescent="0.3">
+      <c r="C41" s="23"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="23"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="24"/>
+      <c r="I41" s="24"/>
+    </row>
+    <row r="42" spans="3:9" ht="30" x14ac:dyDescent="0.3">
+      <c r="C42" s="23"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="23"/>
+      <c r="G42" s="24"/>
+      <c r="H42" s="24"/>
+      <c r="I42" s="24"/>
+    </row>
+    <row r="43" spans="3:9" ht="30" x14ac:dyDescent="0.3">
+      <c r="C43" s="23"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="23"/>
+      <c r="G43" s="24"/>
+      <c r="H43" s="24"/>
+      <c r="I43" s="24"/>
+    </row>
+    <row r="44" spans="3:9" ht="30" x14ac:dyDescent="0.3">
+      <c r="C44" s="23"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="24"/>
+      <c r="H44" s="24"/>
+      <c r="I44" s="24"/>
+    </row>
+    <row r="45" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C45" s="23"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="23"/>
+      <c r="G45" s="24"/>
+      <c r="H45" s="24"/>
+      <c r="I45" s="24"/>
+    </row>
+    <row r="46" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C46" s="23"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="23"/>
+      <c r="G46" s="24"/>
+      <c r="H46" s="24"/>
+      <c r="I46" s="24"/>
+    </row>
+    <row r="47" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C47" s="23"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="24"/>
+      <c r="F47" s="23"/>
+      <c r="G47" s="24"/>
+      <c r="H47" s="24"/>
+      <c r="I47" s="24"/>
+    </row>
+    <row r="48" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C48" s="23"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="23"/>
+      <c r="G48" s="24"/>
+      <c r="H48" s="24"/>
+      <c r="I48" s="24"/>
+    </row>
+    <row r="49" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C49" s="23"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="23"/>
+      <c r="G49" s="24"/>
+      <c r="H49" s="24"/>
+      <c r="I49" s="24"/>
+    </row>
+    <row r="50" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C50" s="23"/>
+      <c r="D50" s="24"/>
+      <c r="E50" s="24"/>
+      <c r="F50" s="23"/>
+      <c r="G50" s="24"/>
+      <c r="H50" s="24"/>
+      <c r="I50" s="24"/>
+    </row>
+    <row r="51" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C51" s="23"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="23"/>
+      <c r="G51" s="24"/>
+      <c r="H51" s="24"/>
+      <c r="I51" s="24"/>
+    </row>
+    <row r="52" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C52" s="23"/>
+      <c r="D52" s="24"/>
+      <c r="E52" s="24"/>
+      <c r="F52" s="23"/>
+      <c r="G52" s="24"/>
+      <c r="H52" s="24"/>
+      <c r="I52" s="24"/>
+    </row>
+    <row r="53" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C53" s="23"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="24"/>
+      <c r="F53" s="23"/>
+      <c r="G53" s="24"/>
+      <c r="H53" s="24"/>
+      <c r="I53" s="24"/>
+    </row>
+    <row r="54" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C54" s="23"/>
+      <c r="D54" s="24"/>
+      <c r="E54" s="24"/>
+      <c r="F54" s="23"/>
+      <c r="G54" s="24"/>
+      <c r="H54" s="24"/>
+      <c r="I54" s="24"/>
+    </row>
+    <row r="55" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C55" s="23"/>
+      <c r="D55" s="24"/>
+      <c r="E55" s="24"/>
+      <c r="F55" s="23"/>
+      <c r="G55" s="24"/>
+      <c r="H55" s="24"/>
+      <c r="I55" s="24"/>
+    </row>
+    <row r="56" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C56" s="23"/>
+      <c r="D56" s="24"/>
+      <c r="E56" s="24"/>
+      <c r="F56" s="23"/>
+      <c r="G56" s="24"/>
+      <c r="H56" s="24"/>
+      <c r="I56" s="24"/>
+    </row>
+    <row r="57" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C57" s="23"/>
+      <c r="D57" s="24"/>
+      <c r="E57" s="24"/>
+      <c r="F57" s="23"/>
+      <c r="G57" s="24"/>
+      <c r="H57" s="24"/>
+      <c r="I57" s="24"/>
+    </row>
+    <row r="58" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C58" s="23"/>
+      <c r="D58" s="24"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="23"/>
+      <c r="G58" s="24"/>
+      <c r="H58" s="24"/>
+      <c r="I58" s="24"/>
+    </row>
+    <row r="59" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C59" s="23"/>
+      <c r="D59" s="24"/>
+      <c r="E59" s="24"/>
+      <c r="F59" s="23"/>
+      <c r="G59" s="24"/>
+      <c r="H59" s="24"/>
+      <c r="I59" s="24"/>
+    </row>
+    <row r="60" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C60" s="23"/>
+      <c r="D60" s="24"/>
+      <c r="E60" s="24"/>
+      <c r="F60" s="23"/>
+      <c r="G60" s="24"/>
+      <c r="H60" s="24"/>
+      <c r="I60" s="24"/>
+    </row>
+    <row r="61" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C61" s="23"/>
+      <c r="D61" s="24"/>
+      <c r="E61" s="24"/>
+      <c r="F61" s="23"/>
+      <c r="G61" s="24"/>
+      <c r="H61" s="24"/>
+      <c r="I61" s="24"/>
+    </row>
+    <row r="62" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C62" s="23"/>
+      <c r="D62" s="24"/>
+      <c r="E62" s="24"/>
+      <c r="F62" s="23"/>
+      <c r="G62" s="24"/>
+      <c r="H62" s="24"/>
+      <c r="I62" s="24"/>
+    </row>
+    <row r="63" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C63" s="23"/>
+      <c r="D63" s="24"/>
+      <c r="E63" s="24"/>
+      <c r="F63" s="23"/>
+      <c r="G63" s="24"/>
+      <c r="H63" s="24"/>
+      <c r="I63" s="24"/>
+    </row>
+    <row r="64" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C64" s="23"/>
+      <c r="D64" s="24"/>
+      <c r="E64" s="24"/>
+      <c r="F64" s="23"/>
+      <c r="G64" s="24"/>
+      <c r="H64" s="24"/>
+      <c r="I64" s="24"/>
+    </row>
+    <row r="65" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C65" s="23"/>
+      <c r="D65" s="24"/>
+      <c r="E65" s="24"/>
+      <c r="F65" s="23"/>
+      <c r="G65" s="24"/>
+      <c r="H65" s="24"/>
+      <c r="I65" s="24"/>
+    </row>
+    <row r="66" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C66" s="23"/>
+      <c r="D66" s="24"/>
+      <c r="E66" s="24"/>
+      <c r="F66" s="23"/>
+      <c r="G66" s="24"/>
+      <c r="H66" s="24"/>
+      <c r="I66" s="24"/>
+    </row>
+    <row r="67" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C67" s="23"/>
+      <c r="D67" s="24"/>
+      <c r="E67" s="24"/>
+      <c r="F67" s="23"/>
+      <c r="G67" s="24"/>
+      <c r="H67" s="24"/>
+      <c r="I67" s="24"/>
+    </row>
+    <row r="68" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C68" s="23"/>
+      <c r="D68" s="24"/>
+      <c r="E68" s="24"/>
+      <c r="F68" s="23"/>
+      <c r="G68" s="24"/>
+      <c r="H68" s="24"/>
+      <c r="I68" s="24"/>
+    </row>
+    <row r="69" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C69" s="23"/>
+      <c r="D69" s="24"/>
+      <c r="E69" s="24"/>
+      <c r="F69" s="23"/>
+      <c r="G69" s="24"/>
+      <c r="H69" s="24"/>
+      <c r="I69" s="24"/>
+    </row>
+    <row r="70" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C70" s="23"/>
+      <c r="D70" s="24"/>
+      <c r="E70" s="24"/>
+      <c r="F70" s="23"/>
+      <c r="G70" s="24"/>
+      <c r="H70" s="24"/>
+      <c r="I70" s="24"/>
+    </row>
+    <row r="71" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C71" s="23"/>
+      <c r="D71" s="24"/>
+      <c r="E71" s="24"/>
+      <c r="F71" s="23"/>
+      <c r="G71" s="24"/>
+      <c r="H71" s="24"/>
+      <c r="I71" s="24"/>
+    </row>
+    <row r="72" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C72" s="23"/>
+      <c r="D72" s="24"/>
+      <c r="E72" s="24"/>
+      <c r="F72" s="23"/>
+      <c r="G72" s="24"/>
+      <c r="H72" s="24"/>
+      <c r="I72" s="24"/>
+    </row>
+    <row r="73" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C73" s="23"/>
+      <c r="D73" s="24"/>
+      <c r="E73" s="24"/>
+      <c r="F73" s="23"/>
+      <c r="G73" s="24"/>
+      <c r="H73" s="24"/>
+      <c r="I73" s="24"/>
+    </row>
+    <row r="74" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C74" s="23"/>
+      <c r="D74" s="24"/>
+      <c r="E74" s="24"/>
+      <c r="F74" s="23"/>
+      <c r="G74" s="24"/>
+      <c r="H74" s="24"/>
+      <c r="I74" s="24"/>
+    </row>
+    <row r="75" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C75" s="23"/>
+      <c r="D75" s="24"/>
+      <c r="E75" s="24"/>
+      <c r="F75" s="23"/>
+      <c r="G75" s="24"/>
+      <c r="H75" s="24"/>
+      <c r="I75" s="24"/>
+    </row>
+    <row r="76" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C76" s="23"/>
+      <c r="D76" s="24"/>
+      <c r="E76" s="24"/>
+      <c r="F76" s="23"/>
+      <c r="G76" s="24"/>
+      <c r="H76" s="24"/>
+      <c r="I76" s="24"/>
+    </row>
+    <row r="77" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C77" s="23"/>
+      <c r="D77" s="24"/>
+      <c r="E77" s="24"/>
+      <c r="F77" s="23"/>
+      <c r="G77" s="24"/>
+      <c r="H77" s="24"/>
+      <c r="I77" s="24"/>
+    </row>
+    <row r="78" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C78" s="23"/>
+      <c r="D78" s="24"/>
+      <c r="E78" s="24"/>
+      <c r="F78" s="23"/>
+      <c r="G78" s="24"/>
+      <c r="H78" s="24"/>
+      <c r="I78" s="24"/>
+    </row>
+    <row r="79" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C79" s="23"/>
+      <c r="D79" s="24"/>
+      <c r="E79" s="24"/>
+      <c r="F79" s="23"/>
+      <c r="G79" s="24"/>
+      <c r="H79" s="24"/>
+      <c r="I79" s="24"/>
+    </row>
+    <row r="80" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C80" s="23"/>
+      <c r="D80" s="24"/>
+      <c r="E80" s="24"/>
+      <c r="F80" s="23"/>
+      <c r="G80" s="24"/>
+      <c r="H80" s="24"/>
+      <c r="I80" s="24"/>
+    </row>
+    <row r="81" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C81" s="23"/>
+      <c r="D81" s="24"/>
+      <c r="E81" s="24"/>
+      <c r="F81" s="23"/>
+      <c r="G81" s="24"/>
+      <c r="H81" s="24"/>
+      <c r="I81" s="24"/>
+    </row>
+    <row r="82" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C82" s="23"/>
+      <c r="D82" s="24"/>
+      <c r="E82" s="24"/>
+      <c r="F82" s="23"/>
+      <c r="G82" s="24"/>
+      <c r="H82" s="24"/>
+      <c r="I82" s="24"/>
+    </row>
+    <row r="83" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C83" s="23"/>
+      <c r="D83" s="24"/>
+      <c r="E83" s="24"/>
+      <c r="F83" s="23"/>
+      <c r="G83" s="24"/>
+      <c r="H83" s="24"/>
+      <c r="I83" s="24"/>
+    </row>
+    <row r="84" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C84" s="23"/>
+      <c r="D84" s="24"/>
+      <c r="E84" s="24"/>
+      <c r="F84" s="23"/>
+      <c r="G84" s="24"/>
+      <c r="H84" s="24"/>
+      <c r="I84" s="24"/>
+    </row>
+    <row r="85" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C85" s="23"/>
+      <c r="D85" s="24"/>
+      <c r="E85" s="24"/>
+      <c r="F85" s="23"/>
+      <c r="G85" s="24"/>
+      <c r="H85" s="24"/>
+      <c r="I85" s="24"/>
+    </row>
+    <row r="86" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C86" s="23"/>
+      <c r="D86" s="24"/>
+      <c r="E86" s="24"/>
+      <c r="F86" s="23"/>
+      <c r="G86" s="24"/>
+      <c r="H86" s="24"/>
+      <c r="I86" s="24"/>
+    </row>
+    <row r="87" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C87" s="23"/>
+      <c r="D87" s="24"/>
+      <c r="E87" s="24"/>
+      <c r="F87" s="23"/>
+      <c r="G87" s="24"/>
+      <c r="H87" s="24"/>
+      <c r="I87" s="24"/>
+    </row>
+    <row r="88" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C88" s="23"/>
+      <c r="D88" s="24"/>
+      <c r="E88" s="24"/>
+      <c r="F88" s="23"/>
+      <c r="G88" s="24"/>
+      <c r="H88" s="24"/>
+      <c r="I88" s="24"/>
+    </row>
+    <row r="89" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C89" s="23"/>
+      <c r="D89" s="24"/>
+      <c r="E89" s="24"/>
+      <c r="F89" s="23"/>
+      <c r="G89" s="24"/>
+      <c r="H89" s="24"/>
+      <c r="I89" s="24"/>
+    </row>
+    <row r="90" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C90" s="23"/>
+      <c r="D90" s="24"/>
+      <c r="E90" s="24"/>
+      <c r="F90" s="23"/>
+      <c r="G90" s="24"/>
+      <c r="H90" s="24"/>
+      <c r="I90" s="24"/>
+    </row>
+    <row r="91" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C91" s="23"/>
+      <c r="D91" s="24"/>
+      <c r="E91" s="24"/>
+      <c r="F91" s="23"/>
+      <c r="G91" s="24"/>
+      <c r="H91" s="24"/>
+      <c r="I91" s="24"/>
+    </row>
+    <row r="92" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C92" s="23"/>
+      <c r="D92" s="24"/>
+      <c r="E92" s="24"/>
+      <c r="F92" s="23"/>
+      <c r="G92" s="24"/>
+      <c r="H92" s="24"/>
+      <c r="I92" s="24"/>
+    </row>
+    <row r="93" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C93" s="23"/>
+      <c r="D93" s="24"/>
+      <c r="E93" s="24"/>
+      <c r="F93" s="23"/>
+      <c r="G93" s="24"/>
+      <c r="H93" s="24"/>
+      <c r="I93" s="24"/>
+    </row>
+    <row r="94" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C94" s="23"/>
+      <c r="D94" s="24"/>
+      <c r="E94" s="24"/>
+      <c r="F94" s="23"/>
+      <c r="G94" s="24"/>
+      <c r="H94" s="24"/>
+      <c r="I94" s="24"/>
+    </row>
+    <row r="95" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C95" s="23"/>
+      <c r="D95" s="24"/>
+      <c r="E95" s="24"/>
+      <c r="F95" s="23"/>
+      <c r="G95" s="24"/>
+      <c r="H95" s="24"/>
+      <c r="I95" s="24"/>
+    </row>
+    <row r="96" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C96" s="23"/>
+      <c r="D96" s="24"/>
+      <c r="E96" s="24"/>
+      <c r="F96" s="23"/>
+      <c r="G96" s="24"/>
+      <c r="H96" s="24"/>
+      <c r="I96" s="24"/>
+    </row>
+    <row r="97" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C97" s="23"/>
+      <c r="D97" s="24"/>
+      <c r="E97" s="24"/>
+      <c r="F97" s="23"/>
+      <c r="G97" s="24"/>
+      <c r="H97" s="24"/>
+      <c r="I97" s="24"/>
+    </row>
+    <row r="98" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C98" s="23"/>
+      <c r="D98" s="24"/>
+      <c r="E98" s="24"/>
+      <c r="F98" s="23"/>
+      <c r="G98" s="24"/>
+      <c r="H98" s="24"/>
+      <c r="I98" s="24"/>
+    </row>
+    <row r="99" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C99" s="23"/>
+      <c r="D99" s="24"/>
+      <c r="E99" s="24"/>
+      <c r="F99" s="23"/>
+      <c r="G99" s="24"/>
+      <c r="H99" s="24"/>
+      <c r="I99" s="24"/>
+    </row>
+    <row r="100" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C100" s="23"/>
+      <c r="D100" s="24"/>
+      <c r="E100" s="24"/>
+      <c r="F100" s="23"/>
+      <c r="G100" s="24"/>
+      <c r="H100" s="24"/>
+      <c r="I100" s="24"/>
+    </row>
+    <row r="101" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C101" s="23"/>
+      <c r="D101" s="24"/>
+      <c r="E101" s="24"/>
+      <c r="F101" s="23"/>
+      <c r="G101" s="24"/>
+      <c r="H101" s="24"/>
+      <c r="I101" s="24"/>
+    </row>
+    <row r="102" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C102" s="23"/>
+      <c r="D102" s="24"/>
+      <c r="E102" s="24"/>
+      <c r="F102" s="23"/>
+      <c r="G102" s="24"/>
+      <c r="H102" s="24"/>
+      <c r="I102" s="24"/>
+    </row>
+    <row r="103" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C103" s="23"/>
+      <c r="D103" s="24"/>
+      <c r="E103" s="24"/>
+      <c r="F103" s="23"/>
+      <c r="G103" s="24"/>
+      <c r="H103" s="24"/>
+      <c r="I103" s="24"/>
+    </row>
+    <row r="104" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C104" s="23"/>
+      <c r="D104" s="24"/>
+      <c r="E104" s="24"/>
+      <c r="F104" s="23"/>
+      <c r="G104" s="24"/>
+      <c r="H104" s="24"/>
+      <c r="I104" s="24"/>
+    </row>
+    <row r="105" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C105" s="23"/>
+      <c r="D105" s="24"/>
+      <c r="E105" s="24"/>
+      <c r="F105" s="23"/>
+      <c r="G105" s="24"/>
+      <c r="H105" s="24"/>
+      <c r="I105" s="24"/>
+    </row>
+    <row r="106" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C106" s="23"/>
+      <c r="D106" s="24"/>
+      <c r="E106" s="24"/>
+      <c r="F106" s="23"/>
+      <c r="G106" s="24"/>
+      <c r="H106" s="24"/>
+      <c r="I106" s="24"/>
+    </row>
+    <row r="107" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C107" s="23"/>
+      <c r="D107" s="24"/>
+      <c r="E107" s="24"/>
+      <c r="F107" s="23"/>
+      <c r="G107" s="24"/>
+      <c r="H107" s="24"/>
+      <c r="I107" s="24"/>
+    </row>
+    <row r="108" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C108" s="23"/>
+      <c r="D108" s="24"/>
+      <c r="E108" s="24"/>
+      <c r="F108" s="23"/>
+      <c r="G108" s="24"/>
+      <c r="H108" s="24"/>
+      <c r="I108" s="24"/>
+    </row>
+    <row r="109" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C109" s="23"/>
+      <c r="D109" s="24"/>
+      <c r="E109" s="24"/>
+      <c r="F109" s="23"/>
+      <c r="G109" s="24"/>
+      <c r="H109" s="24"/>
+      <c r="I109" s="24"/>
+    </row>
+    <row r="110" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C110" s="23"/>
+      <c r="D110" s="24"/>
+      <c r="E110" s="24"/>
+      <c r="F110" s="23"/>
+      <c r="G110" s="24"/>
+      <c r="H110" s="24"/>
+      <c r="I110" s="24"/>
+    </row>
+    <row r="111" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C111" s="23"/>
+      <c r="D111" s="24"/>
+      <c r="E111" s="24"/>
+      <c r="F111" s="23"/>
+      <c r="G111" s="24"/>
+      <c r="H111" s="24"/>
+      <c r="I111" s="24"/>
+    </row>
+    <row r="112" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C112" s="23"/>
+      <c r="D112" s="24"/>
+      <c r="E112" s="24"/>
+      <c r="F112" s="23"/>
+      <c r="G112" s="24"/>
+      <c r="H112" s="24"/>
+      <c r="I112" s="24"/>
+    </row>
+    <row r="113" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C113" s="23"/>
+      <c r="D113" s="24"/>
+      <c r="E113" s="24"/>
+      <c r="F113" s="23"/>
+      <c r="G113" s="24"/>
+      <c r="H113" s="24"/>
+      <c r="I113" s="24"/>
+    </row>
+    <row r="114" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C114" s="23"/>
+      <c r="D114" s="24"/>
+      <c r="E114" s="24"/>
+      <c r="F114" s="23"/>
+      <c r="G114" s="24"/>
+      <c r="H114" s="24"/>
+      <c r="I114" s="24"/>
+    </row>
+    <row r="115" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C115" s="23"/>
+      <c r="D115" s="24"/>
+      <c r="E115" s="24"/>
+      <c r="F115" s="23"/>
+      <c r="G115" s="24"/>
+      <c r="H115" s="24"/>
+      <c r="I115" s="24"/>
+    </row>
+    <row r="116" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C116" s="23"/>
+      <c r="D116" s="24"/>
+      <c r="E116" s="24"/>
+      <c r="F116" s="23"/>
+      <c r="G116" s="24"/>
+      <c r="H116" s="24"/>
+      <c r="I116" s="24"/>
+    </row>
+    <row r="117" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C117" s="23"/>
+      <c r="D117" s="24"/>
+      <c r="E117" s="24"/>
+      <c r="F117" s="23"/>
+      <c r="G117" s="24"/>
+      <c r="H117" s="24"/>
+      <c r="I117" s="24"/>
+    </row>
+    <row r="118" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C118" s="23"/>
+      <c r="D118" s="24"/>
+      <c r="E118" s="24"/>
+      <c r="F118" s="23"/>
+      <c r="G118" s="24"/>
+      <c r="H118" s="24"/>
+      <c r="I118" s="24"/>
+    </row>
+    <row r="119" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C119" s="23"/>
+      <c r="D119" s="24"/>
+      <c r="E119" s="24"/>
+      <c r="F119" s="23"/>
+      <c r="G119" s="24"/>
+      <c r="H119" s="24"/>
+      <c r="I119" s="24"/>
+    </row>
+    <row r="120" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C120" s="23"/>
+      <c r="D120" s="24"/>
+      <c r="E120" s="24"/>
+      <c r="F120" s="23"/>
+      <c r="G120" s="24"/>
+      <c r="H120" s="24"/>
+      <c r="I120" s="24"/>
+    </row>
+    <row r="121" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C121" s="23"/>
+      <c r="D121" s="24"/>
+      <c r="E121" s="24"/>
+      <c r="F121" s="23"/>
+      <c r="G121" s="24"/>
+      <c r="H121" s="24"/>
+      <c r="I121" s="24"/>
+    </row>
+    <row r="122" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C122" s="23"/>
+      <c r="D122" s="24"/>
+      <c r="E122" s="24"/>
+      <c r="F122" s="23"/>
+      <c r="G122" s="24"/>
+      <c r="H122" s="24"/>
+      <c r="I122" s="24"/>
+    </row>
+    <row r="123" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C123" s="23"/>
+      <c r="D123" s="24"/>
+      <c r="E123" s="24"/>
+      <c r="F123" s="23"/>
+      <c r="G123" s="24"/>
+      <c r="H123" s="24"/>
+      <c r="I123" s="24"/>
+    </row>
+    <row r="124" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C124" s="23"/>
+      <c r="D124" s="24"/>
+      <c r="E124" s="24"/>
+      <c r="F124" s="23"/>
+      <c r="G124" s="24"/>
+      <c r="H124" s="24"/>
+      <c r="I124" s="24"/>
+    </row>
+    <row r="125" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C125" s="23"/>
+      <c r="D125" s="24"/>
+      <c r="E125" s="24"/>
+      <c r="F125" s="23"/>
+      <c r="G125" s="24"/>
+      <c r="H125" s="24"/>
+      <c r="I125" s="24"/>
+    </row>
+    <row r="126" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C126" s="23"/>
+      <c r="D126" s="24"/>
+      <c r="E126" s="24"/>
+      <c r="F126" s="23"/>
+      <c r="G126" s="24"/>
+      <c r="H126" s="24"/>
+      <c r="I126" s="24"/>
+    </row>
+    <row r="127" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C127" s="23"/>
+      <c r="D127" s="24"/>
+      <c r="E127" s="24"/>
+      <c r="F127" s="23"/>
+      <c r="G127" s="24"/>
+      <c r="H127" s="24"/>
+      <c r="I127" s="24"/>
+    </row>
+    <row r="128" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C128" s="23"/>
+      <c r="D128" s="24"/>
+      <c r="E128" s="24"/>
+      <c r="F128" s="23"/>
+      <c r="G128" s="24"/>
+      <c r="H128" s="24"/>
+      <c r="I128" s="24"/>
+    </row>
+    <row r="129" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C129" s="23"/>
+      <c r="D129" s="24"/>
+      <c r="E129" s="24"/>
+      <c r="F129" s="23"/>
+      <c r="G129" s="24"/>
+      <c r="H129" s="24"/>
+      <c r="I129" s="24"/>
+    </row>
+    <row r="130" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C130" s="23"/>
+      <c r="D130" s="24"/>
+      <c r="E130" s="24"/>
+      <c r="F130" s="23"/>
+      <c r="G130" s="24"/>
+      <c r="H130" s="24"/>
+      <c r="I130" s="24"/>
+    </row>
+    <row r="131" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C131" s="23"/>
+      <c r="D131" s="24"/>
+      <c r="E131" s="24"/>
+      <c r="F131" s="23"/>
+      <c r="G131" s="24"/>
+      <c r="H131" s="24"/>
+      <c r="I131" s="24"/>
+    </row>
+    <row r="132" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C132" s="23"/>
+      <c r="D132" s="24"/>
+      <c r="E132" s="24"/>
+      <c r="F132" s="23"/>
+      <c r="G132" s="24"/>
+      <c r="H132" s="24"/>
+      <c r="I132" s="24"/>
+    </row>
+    <row r="133" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C133" s="23"/>
+      <c r="D133" s="24"/>
+      <c r="E133" s="24"/>
+      <c r="F133" s="23"/>
+      <c r="G133" s="24"/>
+      <c r="H133" s="24"/>
+      <c r="I133" s="24"/>
+    </row>
+    <row r="134" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C134" s="23"/>
+      <c r="D134" s="24"/>
+      <c r="E134" s="24"/>
+      <c r="F134" s="23"/>
+      <c r="G134" s="24"/>
+      <c r="H134" s="24"/>
+      <c r="I134" s="24"/>
+    </row>
+    <row r="135" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C135" s="23"/>
+      <c r="D135" s="24"/>
+      <c r="E135" s="24"/>
+      <c r="F135" s="23"/>
+      <c r="G135" s="24"/>
+      <c r="H135" s="24"/>
+      <c r="I135" s="24"/>
+    </row>
+    <row r="136" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C136" s="23"/>
+      <c r="D136" s="24"/>
+      <c r="E136" s="24"/>
+      <c r="F136" s="23"/>
+      <c r="G136" s="24"/>
+      <c r="H136" s="24"/>
+      <c r="I136" s="24"/>
+    </row>
+    <row r="137" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C137" s="23"/>
+      <c r="D137" s="24"/>
+      <c r="E137" s="24"/>
+      <c r="F137" s="23"/>
+      <c r="G137" s="24"/>
+      <c r="H137" s="24"/>
+      <c r="I137" s="24"/>
+    </row>
+    <row r="138" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C138" s="23"/>
+      <c r="D138" s="24"/>
+      <c r="E138" s="24"/>
+      <c r="F138" s="23"/>
+      <c r="G138" s="24"/>
+      <c r="H138" s="24"/>
+      <c r="I138" s="24"/>
+    </row>
+    <row r="139" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C139" s="23"/>
+      <c r="D139" s="24"/>
+      <c r="E139" s="24"/>
+      <c r="F139" s="23"/>
+      <c r="G139" s="24"/>
+      <c r="H139" s="24"/>
+      <c r="I139" s="24"/>
+    </row>
+    <row r="140" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C140" s="23"/>
+      <c r="D140" s="24"/>
+      <c r="E140" s="24"/>
+      <c r="F140" s="23"/>
+      <c r="G140" s="24"/>
+      <c r="H140" s="24"/>
+      <c r="I140" s="24"/>
+    </row>
+    <row r="141" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C141" s="23"/>
+      <c r="D141" s="24"/>
+      <c r="E141" s="24"/>
+      <c r="F141" s="23"/>
+      <c r="G141" s="24"/>
+      <c r="H141" s="24"/>
+      <c r="I141" s="24"/>
+    </row>
+    <row r="142" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C142" s="23"/>
+      <c r="D142" s="24"/>
+      <c r="E142" s="24"/>
+      <c r="F142" s="23"/>
+      <c r="G142" s="24"/>
+      <c r="H142" s="24"/>
+      <c r="I142" s="24"/>
+    </row>
+    <row r="143" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C143" s="23"/>
+      <c r="D143" s="24"/>
+      <c r="E143" s="24"/>
+      <c r="F143" s="23"/>
+      <c r="G143" s="24"/>
+      <c r="H143" s="24"/>
+      <c r="I143" s="24"/>
+    </row>
+    <row r="144" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C144" s="23"/>
+      <c r="D144" s="24"/>
+      <c r="E144" s="24"/>
+      <c r="F144" s="23"/>
+      <c r="G144" s="24"/>
+      <c r="H144" s="24"/>
+      <c r="I144" s="24"/>
+    </row>
+    <row r="145" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C145" s="23"/>
+      <c r="D145" s="24"/>
+      <c r="E145" s="24"/>
+      <c r="F145" s="23"/>
+      <c r="G145" s="24"/>
+      <c r="H145" s="24"/>
+      <c r="I145" s="24"/>
+    </row>
+    <row r="146" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C146" s="23"/>
+      <c r="D146" s="24"/>
+      <c r="E146" s="24"/>
+      <c r="F146" s="23"/>
+      <c r="G146" s="24"/>
+      <c r="H146" s="24"/>
+      <c r="I146" s="24"/>
+    </row>
+    <row r="147" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C147" s="23"/>
+      <c r="D147" s="24"/>
+      <c r="E147" s="24"/>
+      <c r="F147" s="23"/>
+      <c r="G147" s="24"/>
+      <c r="H147" s="24"/>
+      <c r="I147" s="24"/>
+    </row>
+    <row r="148" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C148" s="23"/>
+      <c r="D148" s="24"/>
+      <c r="E148" s="24"/>
+      <c r="F148" s="23"/>
+      <c r="G148" s="24"/>
+      <c r="H148" s="24"/>
+      <c r="I148" s="24"/>
+    </row>
+    <row r="149" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C149" s="23"/>
+      <c r="D149" s="24"/>
+      <c r="E149" s="24"/>
+      <c r="F149" s="23"/>
+      <c r="G149" s="24"/>
+      <c r="H149" s="24"/>
+      <c r="I149" s="24"/>
+    </row>
+    <row r="150" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C150" s="23"/>
+      <c r="D150" s="24"/>
+      <c r="E150" s="24"/>
+      <c r="F150" s="23"/>
+      <c r="G150" s="24"/>
+      <c r="H150" s="24"/>
+      <c r="I150" s="24"/>
+    </row>
+    <row r="151" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C151" s="23"/>
+      <c r="D151" s="24"/>
+      <c r="E151" s="24"/>
+      <c r="F151" s="23"/>
+      <c r="G151" s="24"/>
+      <c r="H151" s="24"/>
+      <c r="I151" s="24"/>
+    </row>
+    <row r="152" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C152" s="23"/>
+      <c r="D152" s="24"/>
+      <c r="E152" s="24"/>
+      <c r="F152" s="23"/>
+      <c r="G152" s="24"/>
+      <c r="H152" s="24"/>
+      <c r="I152" s="24"/>
+    </row>
+    <row r="153" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C153" s="23"/>
+      <c r="D153" s="24"/>
+      <c r="E153" s="24"/>
+      <c r="F153" s="23"/>
+      <c r="G153" s="24"/>
+      <c r="H153" s="24"/>
+      <c r="I153" s="24"/>
+    </row>
+    <row r="154" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C154" s="23"/>
+      <c r="D154" s="24"/>
+      <c r="E154" s="24"/>
+      <c r="F154" s="23"/>
+      <c r="G154" s="24"/>
+      <c r="H154" s="24"/>
+      <c r="I154" s="24"/>
+    </row>
+    <row r="155" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C155" s="23"/>
+      <c r="D155" s="24"/>
+      <c r="E155" s="24"/>
+      <c r="F155" s="23"/>
+      <c r="G155" s="24"/>
+      <c r="H155" s="24"/>
+      <c r="I155" s="24"/>
+    </row>
+    <row r="156" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C156" s="23"/>
+      <c r="D156" s="24"/>
+      <c r="E156" s="24"/>
+      <c r="F156" s="23"/>
+      <c r="G156" s="24"/>
+      <c r="H156" s="24"/>
+      <c r="I156" s="24"/>
+    </row>
+    <row r="157" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C157" s="23"/>
+      <c r="D157" s="24"/>
+      <c r="E157" s="24"/>
+      <c r="F157" s="23"/>
+      <c r="G157" s="24"/>
+      <c r="H157" s="24"/>
+      <c r="I157" s="24"/>
+    </row>
+    <row r="158" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C158" s="23"/>
+      <c r="D158" s="24"/>
+      <c r="E158" s="24"/>
+      <c r="F158" s="23"/>
+      <c r="G158" s="24"/>
+      <c r="H158" s="24"/>
+      <c r="I158" s="24"/>
+    </row>
+    <row r="159" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C159" s="23"/>
+      <c r="D159" s="24"/>
+      <c r="E159" s="24"/>
+      <c r="F159" s="23"/>
+      <c r="G159" s="24"/>
+      <c r="H159" s="24"/>
+      <c r="I159" s="24"/>
+    </row>
+    <row r="160" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C160" s="23"/>
+      <c r="D160" s="24"/>
+      <c r="E160" s="24"/>
+      <c r="F160" s="23"/>
+      <c r="G160" s="24"/>
+      <c r="H160" s="24"/>
+      <c r="I160" s="24"/>
+    </row>
+    <row r="161" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C161" s="23"/>
+      <c r="D161" s="24"/>
+      <c r="E161" s="24"/>
+      <c r="F161" s="23"/>
+      <c r="G161" s="24"/>
+      <c r="H161" s="24"/>
+      <c r="I161" s="24"/>
+    </row>
+    <row r="162" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C162" s="23"/>
+      <c r="D162" s="24"/>
+      <c r="E162" s="24"/>
+      <c r="F162" s="23"/>
+      <c r="G162" s="24"/>
+      <c r="H162" s="24"/>
+      <c r="I162" s="24"/>
+    </row>
+    <row r="163" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C163" s="23"/>
+      <c r="D163" s="24"/>
+      <c r="E163" s="24"/>
+      <c r="F163" s="23"/>
+      <c r="G163" s="24"/>
+      <c r="H163" s="24"/>
+      <c r="I163" s="24"/>
+    </row>
+    <row r="164" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C164" s="23"/>
+      <c r="D164" s="24"/>
+      <c r="E164" s="24"/>
+      <c r="F164" s="23"/>
+      <c r="G164" s="24"/>
+      <c r="H164" s="24"/>
+      <c r="I164" s="24"/>
+    </row>
+    <row r="165" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C165" s="23"/>
+      <c r="D165" s="24"/>
+      <c r="E165" s="24"/>
+      <c r="F165" s="23"/>
+      <c r="G165" s="24"/>
+      <c r="H165" s="24"/>
+      <c r="I165" s="24"/>
+    </row>
+    <row r="166" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C166" s="23"/>
+      <c r="D166" s="24"/>
+      <c r="E166" s="24"/>
+      <c r="F166" s="23"/>
+      <c r="G166" s="24"/>
+      <c r="H166" s="24"/>
+      <c r="I166" s="24"/>
+    </row>
+    <row r="167" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C167" s="23"/>
+      <c r="D167" s="24"/>
+      <c r="E167" s="24"/>
+      <c r="F167" s="23"/>
+      <c r="G167" s="24"/>
+      <c r="H167" s="24"/>
+      <c r="I167" s="24"/>
+    </row>
+    <row r="168" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C168" s="23"/>
+      <c r="D168" s="24"/>
+      <c r="E168" s="24"/>
+      <c r="F168" s="23"/>
+      <c r="G168" s="24"/>
+      <c r="H168" s="24"/>
+      <c r="I168" s="24"/>
+    </row>
+    <row r="169" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C169" s="23"/>
+      <c r="D169" s="24"/>
+      <c r="E169" s="24"/>
+      <c r="F169" s="23"/>
+      <c r="G169" s="24"/>
+      <c r="H169" s="24"/>
+      <c r="I169" s="24"/>
+    </row>
+    <row r="170" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C170" s="23"/>
+      <c r="D170" s="24"/>
+      <c r="E170" s="24"/>
+      <c r="F170" s="23"/>
+      <c r="G170" s="24"/>
+      <c r="H170" s="24"/>
+      <c r="I170" s="24"/>
+    </row>
+    <row r="171" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C171" s="23"/>
+      <c r="D171" s="24"/>
+      <c r="E171" s="24"/>
+      <c r="F171" s="23"/>
+      <c r="G171" s="24"/>
+      <c r="H171" s="24"/>
+      <c r="I171" s="24"/>
+    </row>
+    <row r="172" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C172" s="23"/>
+      <c r="D172" s="24"/>
+      <c r="E172" s="24"/>
+      <c r="F172" s="23"/>
+      <c r="G172" s="24"/>
+      <c r="H172" s="24"/>
+      <c r="I172" s="24"/>
+    </row>
+    <row r="173" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C173" s="23"/>
+      <c r="D173" s="24"/>
+      <c r="E173" s="24"/>
+      <c r="F173" s="23"/>
+      <c r="G173" s="24"/>
+      <c r="H173" s="24"/>
+      <c r="I173" s="24"/>
+    </row>
+    <row r="174" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C174" s="23"/>
+      <c r="D174" s="24"/>
+      <c r="E174" s="24"/>
+      <c r="F174" s="23"/>
+      <c r="G174" s="24"/>
+      <c r="H174" s="24"/>
+      <c r="I174" s="24"/>
+    </row>
+    <row r="175" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C175" s="23"/>
+      <c r="D175" s="24"/>
+      <c r="E175" s="24"/>
+      <c r="F175" s="23"/>
+      <c r="G175" s="24"/>
+      <c r="H175" s="24"/>
+      <c r="I175" s="24"/>
+    </row>
+    <row r="176" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C176" s="23"/>
+      <c r="D176" s="24"/>
+      <c r="E176" s="24"/>
+      <c r="F176" s="23"/>
+      <c r="G176" s="24"/>
+      <c r="H176" s="24"/>
+      <c r="I176" s="24"/>
+    </row>
+  </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AD1747D-4C0D-204D-A6FF-B800C7C93043}">
+  <dimension ref="A2:H112"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="18">
+        <v>41471</v>
+      </c>
+      <c r="C3" s="16">
+        <v>2</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="4">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="18">
+        <v>41471</v>
+      </c>
+      <c r="C4" s="16">
+        <v>7</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="17">
+        <v>33</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="4">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="18">
+        <v>41471</v>
+      </c>
+      <c r="C5" s="16">
+        <v>3</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="4">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="18">
+        <v>41471</v>
+      </c>
+      <c r="C6" s="16">
+        <v>1</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="4">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="18">
+        <v>41473</v>
+      </c>
+      <c r="C7" s="16">
+        <v>3</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="17">
+        <v>40</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="4">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="18">
+        <v>41473</v>
+      </c>
+      <c r="C8" s="16">
+        <v>7</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="17">
+        <v>48</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="4">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="18">
+        <v>41473</v>
+      </c>
+      <c r="C9" s="16">
+        <v>4</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="17">
+        <v>29</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="4">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="19">
+        <v>41473</v>
+      </c>
+      <c r="C10" s="20">
+        <v>6</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="21">
+        <v>37</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="4">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+      <c r="A11" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="18">
+        <v>41505</v>
+      </c>
+      <c r="C11" s="16">
+        <v>8</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="17">
+        <v>52</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="24"/>
+    </row>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+      <c r="A12" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="18">
+        <v>41564</v>
+      </c>
+      <c r="C12" s="16">
+        <v>3</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="17">
+        <v>33</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="24"/>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+      <c r="A13" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="18">
+        <v>41564</v>
+      </c>
+      <c r="C13" s="16">
+        <v>3</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="17">
+        <v>50</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="24"/>
+    </row>
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+      <c r="A14" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="18">
+        <v>41618</v>
+      </c>
+      <c r="C14" s="16">
+        <v>9</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="17">
+        <v>40</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="24"/>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+      <c r="A15" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="18">
+        <v>41618</v>
+      </c>
+      <c r="C15" s="16">
+        <v>1</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="17">
+        <v>45</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" s="24"/>
+    </row>
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.3">
+      <c r="A16" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="19">
+        <v>41619</v>
+      </c>
+      <c r="C16" s="20">
+        <v>8</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="21">
+        <v>41</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="24"/>
+    </row>
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.3">
+      <c r="A17" s="23"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+    </row>
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.3">
+      <c r="A18" s="23"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.3">
+      <c r="A19" s="23"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+    </row>
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.3">
+      <c r="A20" s="23"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+    </row>
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.3">
+      <c r="A21" s="23"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+    </row>
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.3">
+      <c r="A22" s="23"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+    </row>
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.3">
+      <c r="A23" s="23"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+    </row>
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.3">
+      <c r="A24" s="23"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+    </row>
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.3">
+      <c r="A25" s="23"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+    </row>
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.3">
+      <c r="A26" s="23"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+    </row>
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.3">
+      <c r="A27" s="23"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+    </row>
+    <row r="28" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A28" s="23"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+    </row>
+    <row r="29" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A29" s="23"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
+    </row>
+    <row r="30" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A30" s="23"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+    </row>
+    <row r="31" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A31" s="23"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+    </row>
+    <row r="32" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A32" s="23"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+    </row>
+    <row r="33" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A33" s="23"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+    </row>
+    <row r="34" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A34" s="23"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+    </row>
+    <row r="35" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A35" s="23"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+    </row>
+    <row r="36" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A36" s="23"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="24"/>
+    </row>
+    <row r="37" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A37" s="23"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="24"/>
+    </row>
+    <row r="38" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A38" s="23"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="24"/>
+    </row>
+    <row r="39" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A39" s="23"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="24"/>
+    </row>
+    <row r="40" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A40" s="23"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="24"/>
+    </row>
+    <row r="41" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A41" s="23"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="24"/>
+    </row>
+    <row r="42" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A42" s="23"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="24"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="24"/>
+    </row>
+    <row r="43" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A43" s="23"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="24"/>
+      <c r="G43" s="24"/>
+    </row>
+    <row r="44" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A44" s="23"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="24"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="24"/>
+      <c r="G44" s="24"/>
+    </row>
+    <row r="45" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A45" s="23"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="24"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="24"/>
+    </row>
+    <row r="46" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A46" s="23"/>
+      <c r="B46" s="24"/>
+      <c r="C46" s="24"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="24"/>
+    </row>
+    <row r="47" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A47" s="23"/>
+      <c r="B47" s="24"/>
+      <c r="C47" s="24"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="24"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="24"/>
+    </row>
+    <row r="48" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A48" s="23"/>
+      <c r="B48" s="24"/>
+      <c r="C48" s="24"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="24"/>
+    </row>
+    <row r="49" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A49" s="23"/>
+      <c r="B49" s="24"/>
+      <c r="C49" s="24"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="24"/>
+    </row>
+    <row r="50" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A50" s="23"/>
+      <c r="B50" s="24"/>
+      <c r="C50" s="24"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="24"/>
+      <c r="F50" s="24"/>
+      <c r="G50" s="24"/>
+    </row>
+    <row r="51" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A51" s="23"/>
+      <c r="B51" s="24"/>
+      <c r="C51" s="24"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="24"/>
+      <c r="G51" s="24"/>
+    </row>
+    <row r="52" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A52" s="23"/>
+      <c r="B52" s="24"/>
+      <c r="C52" s="24"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="24"/>
+      <c r="F52" s="24"/>
+      <c r="G52" s="24"/>
+    </row>
+    <row r="53" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A53" s="23"/>
+      <c r="B53" s="24"/>
+      <c r="C53" s="24"/>
+      <c r="D53" s="23"/>
+      <c r="E53" s="24"/>
+      <c r="F53" s="24"/>
+      <c r="G53" s="24"/>
+    </row>
+    <row r="54" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A54" s="23"/>
+      <c r="B54" s="24"/>
+      <c r="C54" s="24"/>
+      <c r="D54" s="23"/>
+      <c r="E54" s="24"/>
+      <c r="F54" s="24"/>
+      <c r="G54" s="24"/>
+    </row>
+    <row r="55" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A55" s="23"/>
+      <c r="B55" s="24"/>
+      <c r="C55" s="24"/>
+      <c r="D55" s="23"/>
+      <c r="E55" s="24"/>
+      <c r="F55" s="24"/>
+      <c r="G55" s="24"/>
+    </row>
+    <row r="56" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A56" s="23"/>
+      <c r="B56" s="24"/>
+      <c r="C56" s="24"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="24"/>
+      <c r="F56" s="24"/>
+      <c r="G56" s="24"/>
+    </row>
+    <row r="57" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A57" s="23"/>
+      <c r="B57" s="24"/>
+      <c r="C57" s="24"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="24"/>
+      <c r="F57" s="24"/>
+      <c r="G57" s="24"/>
+    </row>
+    <row r="58" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A58" s="23"/>
+      <c r="B58" s="24"/>
+      <c r="C58" s="24"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="24"/>
+    </row>
+    <row r="59" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A59" s="23"/>
+      <c r="B59" s="24"/>
+      <c r="C59" s="24"/>
+      <c r="D59" s="23"/>
+      <c r="E59" s="24"/>
+      <c r="F59" s="24"/>
+      <c r="G59" s="24"/>
+    </row>
+    <row r="60" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A60" s="23"/>
+      <c r="B60" s="24"/>
+      <c r="C60" s="24"/>
+      <c r="D60" s="23"/>
+      <c r="E60" s="24"/>
+      <c r="F60" s="24"/>
+      <c r="G60" s="24"/>
+    </row>
+    <row r="61" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A61" s="23"/>
+      <c r="B61" s="24"/>
+      <c r="C61" s="24"/>
+      <c r="D61" s="23"/>
+      <c r="E61" s="24"/>
+      <c r="F61" s="24"/>
+      <c r="G61" s="24"/>
+    </row>
+    <row r="62" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A62" s="23"/>
+      <c r="B62" s="24"/>
+      <c r="C62" s="24"/>
+      <c r="D62" s="23"/>
+      <c r="E62" s="24"/>
+      <c r="F62" s="24"/>
+      <c r="G62" s="24"/>
+    </row>
+    <row r="63" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A63" s="23"/>
+      <c r="B63" s="24"/>
+      <c r="C63" s="24"/>
+      <c r="D63" s="23"/>
+      <c r="E63" s="24"/>
+      <c r="F63" s="24"/>
+      <c r="G63" s="24"/>
+    </row>
+    <row r="64" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A64" s="23"/>
+      <c r="B64" s="24"/>
+      <c r="C64" s="24"/>
+      <c r="D64" s="23"/>
+      <c r="E64" s="24"/>
+      <c r="F64" s="24"/>
+      <c r="G64" s="24"/>
+    </row>
+    <row r="65" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A65" s="23"/>
+      <c r="B65" s="24"/>
+      <c r="C65" s="24"/>
+      <c r="D65" s="23"/>
+      <c r="E65" s="24"/>
+      <c r="F65" s="24"/>
+      <c r="G65" s="24"/>
+    </row>
+    <row r="66" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A66" s="23"/>
+      <c r="B66" s="24"/>
+      <c r="C66" s="24"/>
+      <c r="D66" s="23"/>
+      <c r="E66" s="24"/>
+      <c r="F66" s="24"/>
+      <c r="G66" s="24"/>
+    </row>
+    <row r="67" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A67" s="23"/>
+      <c r="B67" s="24"/>
+      <c r="C67" s="24"/>
+      <c r="D67" s="23"/>
+      <c r="E67" s="24"/>
+      <c r="F67" s="24"/>
+      <c r="G67" s="24"/>
+    </row>
+    <row r="68" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A68" s="23"/>
+      <c r="B68" s="24"/>
+      <c r="C68" s="24"/>
+      <c r="D68" s="23"/>
+      <c r="E68" s="24"/>
+      <c r="F68" s="24"/>
+      <c r="G68" s="24"/>
+    </row>
+    <row r="69" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A69" s="23"/>
+      <c r="B69" s="24"/>
+      <c r="C69" s="24"/>
+      <c r="D69" s="23"/>
+      <c r="E69" s="24"/>
+      <c r="F69" s="24"/>
+      <c r="G69" s="24"/>
+    </row>
+    <row r="70" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A70" s="23"/>
+      <c r="B70" s="24"/>
+      <c r="C70" s="24"/>
+      <c r="D70" s="23"/>
+      <c r="E70" s="24"/>
+      <c r="F70" s="24"/>
+      <c r="G70" s="24"/>
+    </row>
+    <row r="71" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A71" s="23"/>
+      <c r="B71" s="24"/>
+      <c r="C71" s="24"/>
+      <c r="D71" s="23"/>
+      <c r="E71" s="24"/>
+      <c r="F71" s="24"/>
+      <c r="G71" s="24"/>
+    </row>
+    <row r="72" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A72" s="23"/>
+      <c r="B72" s="24"/>
+      <c r="C72" s="24"/>
+      <c r="D72" s="23"/>
+      <c r="E72" s="24"/>
+      <c r="F72" s="24"/>
+      <c r="G72" s="24"/>
+    </row>
+    <row r="73" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A73" s="23"/>
+      <c r="B73" s="24"/>
+      <c r="C73" s="24"/>
+      <c r="D73" s="23"/>
+      <c r="E73" s="24"/>
+      <c r="F73" s="24"/>
+      <c r="G73" s="24"/>
+    </row>
+    <row r="74" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A74" s="23"/>
+      <c r="B74" s="24"/>
+      <c r="C74" s="24"/>
+      <c r="D74" s="23"/>
+      <c r="E74" s="24"/>
+      <c r="F74" s="24"/>
+      <c r="G74" s="24"/>
+    </row>
+    <row r="75" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A75" s="23"/>
+      <c r="B75" s="24"/>
+      <c r="C75" s="24"/>
+      <c r="D75" s="23"/>
+      <c r="E75" s="24"/>
+      <c r="F75" s="24"/>
+      <c r="G75" s="24"/>
+    </row>
+    <row r="76" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A76" s="23"/>
+      <c r="B76" s="24"/>
+      <c r="C76" s="24"/>
+      <c r="D76" s="23"/>
+      <c r="E76" s="24"/>
+      <c r="F76" s="24"/>
+      <c r="G76" s="24"/>
+    </row>
+    <row r="77" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A77" s="23"/>
+      <c r="B77" s="24"/>
+      <c r="C77" s="24"/>
+      <c r="D77" s="23"/>
+      <c r="E77" s="24"/>
+      <c r="F77" s="24"/>
+      <c r="G77" s="24"/>
+    </row>
+    <row r="78" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A78" s="23"/>
+      <c r="B78" s="24"/>
+      <c r="C78" s="24"/>
+      <c r="D78" s="23"/>
+      <c r="E78" s="24"/>
+      <c r="F78" s="24"/>
+      <c r="G78" s="24"/>
+    </row>
+    <row r="79" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A79" s="23"/>
+      <c r="B79" s="24"/>
+      <c r="C79" s="24"/>
+      <c r="D79" s="23"/>
+      <c r="E79" s="24"/>
+      <c r="F79" s="24"/>
+      <c r="G79" s="24"/>
+    </row>
+    <row r="80" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A80" s="23"/>
+      <c r="B80" s="24"/>
+      <c r="C80" s="24"/>
+      <c r="D80" s="23"/>
+      <c r="E80" s="24"/>
+      <c r="F80" s="24"/>
+      <c r="G80" s="24"/>
+    </row>
+    <row r="81" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A81" s="23"/>
+      <c r="B81" s="24"/>
+      <c r="C81" s="24"/>
+      <c r="D81" s="23"/>
+      <c r="E81" s="24"/>
+      <c r="F81" s="24"/>
+      <c r="G81" s="24"/>
+    </row>
+    <row r="82" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A82" s="23"/>
+      <c r="B82" s="24"/>
+      <c r="C82" s="24"/>
+      <c r="D82" s="23"/>
+      <c r="E82" s="24"/>
+      <c r="F82" s="24"/>
+      <c r="G82" s="24"/>
+    </row>
+    <row r="83" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A83" s="23"/>
+      <c r="B83" s="24"/>
+      <c r="C83" s="24"/>
+      <c r="D83" s="23"/>
+      <c r="E83" s="24"/>
+      <c r="F83" s="24"/>
+      <c r="G83" s="24"/>
+    </row>
+    <row r="84" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A84" s="23"/>
+      <c r="B84" s="24"/>
+      <c r="C84" s="24"/>
+      <c r="D84" s="23"/>
+      <c r="E84" s="24"/>
+      <c r="F84" s="24"/>
+      <c r="G84" s="24"/>
+    </row>
+    <row r="85" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A85" s="23"/>
+      <c r="B85" s="24"/>
+      <c r="C85" s="24"/>
+      <c r="D85" s="23"/>
+      <c r="E85" s="24"/>
+      <c r="F85" s="24"/>
+      <c r="G85" s="24"/>
+    </row>
+    <row r="86" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A86" s="23"/>
+      <c r="B86" s="24"/>
+      <c r="C86" s="24"/>
+      <c r="D86" s="23"/>
+      <c r="E86" s="24"/>
+      <c r="F86" s="24"/>
+      <c r="G86" s="24"/>
+    </row>
+    <row r="87" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A87" s="23"/>
+      <c r="B87" s="24"/>
+      <c r="C87" s="24"/>
+      <c r="D87" s="23"/>
+      <c r="E87" s="24"/>
+      <c r="F87" s="24"/>
+      <c r="G87" s="24"/>
+    </row>
+    <row r="88" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A88" s="23"/>
+      <c r="B88" s="24"/>
+      <c r="C88" s="24"/>
+      <c r="D88" s="23"/>
+      <c r="E88" s="24"/>
+      <c r="F88" s="24"/>
+      <c r="G88" s="24"/>
+    </row>
+    <row r="89" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A89" s="23"/>
+      <c r="B89" s="24"/>
+      <c r="C89" s="24"/>
+      <c r="D89" s="23"/>
+      <c r="E89" s="24"/>
+      <c r="F89" s="24"/>
+      <c r="G89" s="24"/>
+    </row>
+    <row r="90" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A90" s="23"/>
+      <c r="B90" s="24"/>
+      <c r="C90" s="24"/>
+      <c r="D90" s="23"/>
+      <c r="E90" s="24"/>
+      <c r="F90" s="24"/>
+      <c r="G90" s="24"/>
+    </row>
+    <row r="91" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A91" s="23"/>
+      <c r="B91" s="24"/>
+      <c r="C91" s="24"/>
+      <c r="D91" s="23"/>
+      <c r="E91" s="24"/>
+      <c r="F91" s="24"/>
+      <c r="G91" s="24"/>
+    </row>
+    <row r="92" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A92" s="23"/>
+      <c r="B92" s="24"/>
+      <c r="C92" s="24"/>
+      <c r="D92" s="23"/>
+      <c r="E92" s="24"/>
+      <c r="F92" s="24"/>
+      <c r="G92" s="24"/>
+    </row>
+    <row r="93" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A93" s="23"/>
+      <c r="B93" s="24"/>
+      <c r="C93" s="24"/>
+      <c r="D93" s="23"/>
+      <c r="E93" s="24"/>
+      <c r="F93" s="24"/>
+      <c r="G93" s="24"/>
+    </row>
+    <row r="94" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A94" s="23"/>
+      <c r="B94" s="24"/>
+      <c r="C94" s="24"/>
+      <c r="D94" s="23"/>
+      <c r="E94" s="24"/>
+      <c r="F94" s="24"/>
+      <c r="G94" s="24"/>
+    </row>
+    <row r="95" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A95" s="23"/>
+      <c r="B95" s="24"/>
+      <c r="C95" s="24"/>
+      <c r="D95" s="23"/>
+      <c r="E95" s="24"/>
+      <c r="F95" s="24"/>
+      <c r="G95" s="24"/>
+    </row>
+    <row r="96" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A96" s="23"/>
+      <c r="B96" s="24"/>
+      <c r="C96" s="24"/>
+      <c r="D96" s="23"/>
+      <c r="E96" s="24"/>
+      <c r="F96" s="24"/>
+      <c r="G96" s="24"/>
+    </row>
+    <row r="97" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A97" s="23"/>
+      <c r="B97" s="24"/>
+      <c r="C97" s="24"/>
+      <c r="D97" s="23"/>
+      <c r="E97" s="24"/>
+      <c r="F97" s="24"/>
+      <c r="G97" s="24"/>
+    </row>
+    <row r="98" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A98" s="23"/>
+      <c r="B98" s="24"/>
+      <c r="C98" s="24"/>
+      <c r="D98" s="23"/>
+      <c r="E98" s="24"/>
+      <c r="F98" s="24"/>
+      <c r="G98" s="24"/>
+    </row>
+    <row r="99" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A99" s="23"/>
+      <c r="B99" s="24"/>
+      <c r="C99" s="24"/>
+      <c r="D99" s="23"/>
+      <c r="E99" s="24"/>
+      <c r="F99" s="24"/>
+      <c r="G99" s="24"/>
+    </row>
+    <row r="100" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A100" s="23"/>
+      <c r="B100" s="24"/>
+      <c r="C100" s="24"/>
+      <c r="D100" s="23"/>
+      <c r="E100" s="24"/>
+      <c r="F100" s="24"/>
+      <c r="G100" s="24"/>
+    </row>
+    <row r="101" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A101" s="23"/>
+      <c r="B101" s="24"/>
+      <c r="C101" s="24"/>
+      <c r="D101" s="23"/>
+      <c r="E101" s="24"/>
+      <c r="F101" s="24"/>
+      <c r="G101" s="24"/>
+    </row>
+    <row r="102" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A102" s="23"/>
+      <c r="B102" s="24"/>
+      <c r="C102" s="24"/>
+      <c r="D102" s="23"/>
+      <c r="E102" s="24"/>
+      <c r="F102" s="24"/>
+      <c r="G102" s="24"/>
+    </row>
+    <row r="103" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A103" s="23"/>
+      <c r="B103" s="24"/>
+      <c r="C103" s="24"/>
+      <c r="D103" s="23"/>
+      <c r="E103" s="24"/>
+      <c r="F103" s="24"/>
+      <c r="G103" s="24"/>
+    </row>
+    <row r="104" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A104" s="23"/>
+      <c r="B104" s="24"/>
+      <c r="C104" s="24"/>
+      <c r="D104" s="23"/>
+      <c r="E104" s="24"/>
+      <c r="F104" s="24"/>
+      <c r="G104" s="24"/>
+    </row>
+    <row r="105" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A105" s="23"/>
+      <c r="B105" s="24"/>
+      <c r="C105" s="24"/>
+      <c r="D105" s="23"/>
+      <c r="E105" s="24"/>
+      <c r="F105" s="24"/>
+      <c r="G105" s="24"/>
+    </row>
+    <row r="106" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A106" s="23"/>
+      <c r="B106" s="24"/>
+      <c r="C106" s="24"/>
+      <c r="D106" s="23"/>
+      <c r="E106" s="24"/>
+      <c r="F106" s="24"/>
+      <c r="G106" s="24"/>
+    </row>
+    <row r="107" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A107" s="23"/>
+      <c r="B107" s="24"/>
+      <c r="C107" s="24"/>
+      <c r="D107" s="23"/>
+      <c r="E107" s="24"/>
+      <c r="F107" s="24"/>
+      <c r="G107" s="24"/>
+    </row>
+    <row r="108" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A108" s="23"/>
+      <c r="B108" s="24"/>
+      <c r="C108" s="24"/>
+      <c r="D108" s="23"/>
+      <c r="E108" s="24"/>
+      <c r="F108" s="24"/>
+      <c r="G108" s="24"/>
+    </row>
+    <row r="109" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A109" s="23"/>
+      <c r="B109" s="24"/>
+      <c r="C109" s="24"/>
+      <c r="D109" s="23"/>
+      <c r="E109" s="24"/>
+      <c r="F109" s="24"/>
+      <c r="G109" s="24"/>
+    </row>
+    <row r="110" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A110" s="23"/>
+      <c r="B110" s="24"/>
+      <c r="C110" s="24"/>
+      <c r="D110" s="23"/>
+      <c r="E110" s="24"/>
+      <c r="F110" s="24"/>
+      <c r="G110" s="24"/>
+    </row>
+    <row r="111" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A111" s="23"/>
+      <c r="B111" s="24"/>
+      <c r="C111" s="24"/>
+      <c r="D111" s="23"/>
+      <c r="E111" s="24"/>
+      <c r="F111" s="24"/>
+      <c r="G111" s="24"/>
+    </row>
+    <row r="112" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A112" s="23"/>
+      <c r="B112" s="24"/>
+      <c r="C112" s="24"/>
+      <c r="D112" s="23"/>
+      <c r="E112" s="24"/>
+      <c r="F112" s="24"/>
+      <c r="G112" s="24"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="C2:S47"/>
+  <sheetViews>
+    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="25" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="45.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="11.5" style="1"/>
+    <col min="8" max="8" width="22.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.1640625" style="1" customWidth="1"/>
+    <col min="10" max="12" width="11.5" style="1"/>
+    <col min="13" max="13" width="22.5" style="1" customWidth="1"/>
+    <col min="14" max="14" width="20.1640625" style="1" customWidth="1"/>
+    <col min="15" max="19" width="11.5" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:17" ht="69" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+      <c r="C6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="5"/>
+    </row>
+    <row r="7" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+      <c r="C7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" s="5"/>
+      <c r="M7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q7" s="5"/>
+    </row>
+    <row r="8" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+      <c r="C8" s="6">
+        <v>41648</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
+        <v>40</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="6">
+        <v>41647</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="7">
+        <v>42074</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P8" s="4">
+        <v>8</v>
+      </c>
+      <c r="Q8" s="5"/>
+    </row>
+    <row r="9" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+      <c r="C9" s="6">
+        <v>41648</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="4">
+        <v>36</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="6">
+        <v>41647</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K9" s="4">
+        <v>44</v>
+      </c>
+      <c r="L9" s="5"/>
+      <c r="M9" s="7">
+        <v>42102</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="5"/>
+    </row>
+    <row r="10" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+      <c r="C10" s="6">
+        <v>41711</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="4">
+        <v>51</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="6">
+        <v>41647</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" s="4">
+        <v>7</v>
+      </c>
+      <c r="L10" s="5"/>
+      <c r="M10" s="7">
+        <v>42130</v>
+      </c>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="5"/>
+    </row>
+    <row r="11" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+      <c r="C11" s="6">
+        <v>41711</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="4">
+        <v>44</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="6">
+        <v>41647</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K11" s="4">
+        <v>45</v>
+      </c>
+      <c r="L11" s="5"/>
+      <c r="M11" s="7">
+        <v>42142</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="P11" s="4">
+        <v>182</v>
+      </c>
+      <c r="Q11" s="5"/>
+    </row>
+    <row r="12" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+      <c r="C12" s="6">
+        <v>41711</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="4">
+        <v>146</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="6">
+        <v>41647</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="7">
+        <v>42164</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="P12" s="4">
+        <v>29</v>
+      </c>
+      <c r="Q12" s="5"/>
+    </row>
+    <row r="13" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="6">
+        <v>41647</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K13" s="10">
+        <v>157</v>
+      </c>
+      <c r="L13" s="5"/>
+      <c r="M13" s="7">
+        <v>42193</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="P13" s="4">
+        <v>115</v>
+      </c>
+      <c r="Q13" s="5"/>
+    </row>
+    <row r="14" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="6">
+        <v>41647</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="7">
+        <v>42193</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P14" s="4">
+        <v>190</v>
+      </c>
+      <c r="Q14" s="5"/>
+    </row>
+    <row r="15" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="6">
+        <v>41688</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K15" s="10">
+        <v>218</v>
+      </c>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+    </row>
+    <row r="16" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="6">
+        <v>41688</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K16" s="4">
+        <v>7</v>
+      </c>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+    </row>
+    <row r="17" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="6">
+        <v>41688</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K17" s="4">
+        <v>52</v>
+      </c>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+    </row>
+    <row r="18" spans="3:17" ht="30" x14ac:dyDescent="0.3">
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+    </row>
+    <row r="19" spans="3:17" ht="30" x14ac:dyDescent="0.3">
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -1340,556 +4774,6 @@
       <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
     </row>
-    <row r="22" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="5"/>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="5"/>
-    </row>
-    <row r="23" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="G23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
-      <c r="O23" s="5"/>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="5"/>
-    </row>
-    <row r="24" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="G24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="5"/>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="5"/>
-    </row>
-    <row r="25" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="G25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="Q25" s="5"/>
-    </row>
-    <row r="26" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="G26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="Q26" s="5"/>
-    </row>
-    <row r="27" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="G27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="Q27" s="5"/>
-    </row>
-    <row r="28" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="G28" s="5"/>
-      <c r="L28" s="5"/>
-      <c r="Q28" s="5"/>
-    </row>
-  </sheetData>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter alignWithMargins="0">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="C2:S47"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="25" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="22.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.1640625" style="1" customWidth="1"/>
-    <col min="5" max="7" width="11.5" style="1"/>
-    <col min="8" max="8" width="22.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.1640625" style="1" customWidth="1"/>
-    <col min="10" max="12" width="11.5" style="1"/>
-    <col min="13" max="13" width="22.5" style="1" customWidth="1"/>
-    <col min="14" max="14" width="20.1640625" style="1" customWidth="1"/>
-    <col min="15" max="19" width="11.5" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="3:17" ht="69" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="5"/>
-    </row>
-    <row r="7" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L7" s="5"/>
-      <c r="M7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="N7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="P7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q7" s="5"/>
-    </row>
-    <row r="8" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C8" s="6">
-        <v>41648</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="4">
-        <v>40</v>
-      </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="6">
-        <v>41647</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="7">
-        <v>42074</v>
-      </c>
-      <c r="N8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="O8" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P8" s="4">
-        <v>8</v>
-      </c>
-      <c r="Q8" s="5"/>
-    </row>
-    <row r="9" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C9" s="6">
-        <v>41648</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="4">
-        <v>36</v>
-      </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="6">
-        <v>41647</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="K9" s="4">
-        <v>44</v>
-      </c>
-      <c r="L9" s="5"/>
-      <c r="M9" s="7">
-        <v>42102</v>
-      </c>
-      <c r="N9" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="O9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="5"/>
-    </row>
-    <row r="10" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C10" s="6">
-        <v>41711</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="4">
-        <v>51</v>
-      </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="6">
-        <v>41647</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K10" s="4">
-        <v>7</v>
-      </c>
-      <c r="L10" s="5"/>
-      <c r="M10" s="7">
-        <v>42130</v>
-      </c>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="5"/>
-    </row>
-    <row r="11" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C11" s="6">
-        <v>41711</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" s="4">
-        <v>44</v>
-      </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="6">
-        <v>41647</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="K11" s="4">
-        <v>45</v>
-      </c>
-      <c r="L11" s="5"/>
-      <c r="M11" s="7">
-        <v>42142</v>
-      </c>
-      <c r="N11" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="O11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="P11" s="4">
-        <v>182</v>
-      </c>
-      <c r="Q11" s="5"/>
-    </row>
-    <row r="12" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C12" s="6">
-        <v>41711</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" s="4">
-        <v>146</v>
-      </c>
-      <c r="G12" s="5"/>
-      <c r="H12" s="6">
-        <v>41647</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="7">
-        <v>42164</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="O12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="P12" s="4">
-        <v>29</v>
-      </c>
-      <c r="Q12" s="5"/>
-    </row>
-    <row r="13" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="6">
-        <v>41647</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="K13" s="10">
-        <v>157</v>
-      </c>
-      <c r="L13" s="5"/>
-      <c r="M13" s="7">
-        <v>42193</v>
-      </c>
-      <c r="N13" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="O13" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="P13" s="4">
-        <v>115</v>
-      </c>
-      <c r="Q13" s="5"/>
-    </row>
-    <row r="14" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="6">
-        <v>41647</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="7">
-        <v>42193</v>
-      </c>
-      <c r="N14" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="O14" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P14" s="4">
-        <v>190</v>
-      </c>
-      <c r="Q14" s="5"/>
-    </row>
-    <row r="15" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="6">
-        <v>41688</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="K15" s="10">
-        <v>218</v>
-      </c>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
-    </row>
-    <row r="16" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="6">
-        <v>41688</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K16" s="4">
-        <v>7</v>
-      </c>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
-    </row>
-    <row r="17" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="6">
-        <v>41688</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="K17" s="4">
-        <v>52</v>
-      </c>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-    </row>
-    <row r="18" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="5"/>
-    </row>
-    <row r="19" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-    </row>
-    <row r="20" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="5"/>
-    </row>
-    <row r="21" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="5"/>
-    </row>
     <row r="22" spans="3:17" ht="31" x14ac:dyDescent="0.35">
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>

</xml_diff>